<commit_message>
Bring up to date with local development version as of 2024-01-29
</commit_message>
<xml_diff>
--- a/Prosjektregnskap KrUltraCR.xlsx
+++ b/Prosjektregnskap KrUltraCR.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27126"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/16b2c794ae8557f5/Documents/KrUltra/CR/v2/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/16b2c794ae8557f5/Documents/KrUltra/CR - Checkpoint Registration/v2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="239" documentId="11_AD4D1D646341095ACB7000AE0DDF40365ADEDD81" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5CCFFB4D-7F3B-4F9C-8B1D-76C48E6D84ED}"/>
+  <xr:revisionPtr revIDLastSave="242" documentId="11_AD4D1D646341095ACB7000AE0DDF40365ADEDD81" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{20BF2CCE-9233-430E-8274-A0690EFA5FC0}"/>
   <bookViews>
-    <workbookView xWindow="-53" yWindow="-53" windowWidth="25706" windowHeight="15506" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="31515" yWindow="-21720" windowWidth="26040" windowHeight="21840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
@@ -359,15 +359,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>270933</xdr:colOff>
+      <xdr:colOff>219075</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>296334</xdr:rowOff>
+      <xdr:rowOff>447676</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>143943</xdr:colOff>
+      <xdr:colOff>94202</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>105844</xdr:rowOff>
+      <xdr:rowOff>85736</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -397,8 +397,8 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="9584266" y="1024467"/>
-          <a:ext cx="516467" cy="351367"/>
+          <a:off x="9534525" y="1533526"/>
+          <a:ext cx="522827" cy="352435"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -428,7 +428,7 @@
       <xdr:col>10</xdr:col>
       <xdr:colOff>190499</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>55033</xdr:rowOff>
+      <xdr:rowOff>57150</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -481,15 +481,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>279400</xdr:colOff>
+      <xdr:colOff>200025</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>276225</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>152400</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -519,8 +519,8 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="9592733" y="1274233"/>
-          <a:ext cx="516467" cy="478367"/>
+          <a:off x="9515475" y="2076450"/>
+          <a:ext cx="523875" cy="476250"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -550,7 +550,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>38100</xdr:colOff>
       <xdr:row>16</xdr:row>
-      <xdr:rowOff>97366</xdr:rowOff>
+      <xdr:rowOff>95249</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -610,9 +610,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>427554</xdr:colOff>
+      <xdr:colOff>428612</xdr:colOff>
       <xdr:row>9</xdr:row>
-      <xdr:rowOff>237057</xdr:rowOff>
+      <xdr:rowOff>238115</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -931,7 +931,7 @@
   <dimension ref="A1:H51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L18" sqref="L18"/>
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.9375" defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -1031,7 +1031,7 @@
       </c>
       <c r="H4" s="16"/>
     </row>
-    <row r="5" spans="1:8" ht="28.7" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:8" ht="42.35" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A5" s="10" t="s">
         <v>10</v>
       </c>

</xml_diff>